<commit_message>
learn vba git mysql
</commit_message>
<xml_diff>
--- a/study.xlsx
+++ b/study.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>课程</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -281,6 +281,41 @@
   </si>
   <si>
     <t>多邻国（英语）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>角色变量</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -346,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -367,6 +402,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -671,10 +708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -682,9 +719,10 @@
     <col min="2" max="2" width="30.625" customWidth="1"/>
     <col min="3" max="3" width="5.625" customWidth="1"/>
     <col min="4" max="4" width="15.625" customWidth="1"/>
+    <col min="5" max="12" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -695,107 +733,192 @@
       <c r="D1" s="6">
         <v>43590</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+      <c r="E1" s="6">
+        <v>43591</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+    </row>
+    <row r="3" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+    </row>
+    <row r="4" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+    </row>
+    <row r="5" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="8" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+      <c r="E5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+    </row>
+    <row r="6" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="7"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+      <c r="D6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+    </row>
+    <row r="7" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="7"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+      <c r="D7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+    </row>
+    <row r="8" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+    </row>
+    <row r="9" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+    </row>
+    <row r="10" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+    </row>
+    <row r="11" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -804,18 +927,34 @@
       <c r="D11" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+    </row>
+    <row r="12" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="9"/>
       <c r="D12" s="7" t="s">
         <v>26</v>
       </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>